<commit_message>
Se añadió una validación para Excel
</commit_message>
<xml_diff>
--- a/src/Tenis.xlsx
+++ b/src/Tenis.xlsx
@@ -145,7 +145,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -181,7 +181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -209,7 +209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -251,7 +251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -293,7 +293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>